<commit_message>
Peter - updated solvers list and excel
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/Peter-SolverSolutions.xlsx
+++ b/StateOfPractice/Peter-Notes/Peter-SolverSolutions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="249">
   <si>
     <t xml:space="preserve">Sfwr Name</t>
   </si>
@@ -224,6 +224,42 @@
     <t xml:space="preserve">Java Development Toolkit,  Paraview and VMD</t>
   </si>
   <si>
+    <t xml:space="preserve">elbe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuhh.de/elbe/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">efficient academic flow solver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1D, 2D, 3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1Q3, D2Q9, D3Q19, D3Q27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NVIDIA CUDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eLBM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.swmath.org/software/31183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simulation of pore-scale two-phase visco-capillary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESPResSo</t>
   </si>
   <si>
@@ -233,9 +269,6 @@
     <t xml:space="preserve">Molecular Dynamics many-particle simulations</t>
   </si>
   <si>
-    <t xml:space="preserve">3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">D3Q19</t>
   </si>
   <si>
@@ -353,6 +386,69 @@
     <t xml:space="preserve">MIT "Expat"</t>
   </si>
   <si>
+    <t xml:space="preserve">LB2D_Prime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://faculty.fiu.edu/~sukopm/LBnD_Prime/LBnD_Prime.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complementary to the text “LatticeBoltzmannModeling”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORTRAN90, Python, C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LB3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://ccs.chem.ucl.ac.uk/lb3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shan-Chen model for binary fluid interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORTRAN 90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGPL version 3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBM-EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.swmath.org/software/14031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cardiac electrophysiology simulation from 3D images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q5, D3Q7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lbmpy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pypi.org/project/lbmpy/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run fast fluid simulations based on the lattice Boltzmann method in Python on CPUs and GPUs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python, C, CUDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBSim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015 – Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/noirb/lbsim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supporting complex boundaries</t>
+  </si>
+  <si>
     <t xml:space="preserve">lettuce</t>
   </si>
   <si>
@@ -374,60 +470,6 @@
     <t xml:space="preserve">Conda, Python</t>
   </si>
   <si>
-    <t xml:space="preserve">LB2D_Prime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://faculty.fiu.edu/~sukopm/LBnD_Prime/LBnD_Prime.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complementary to the text “LatticeBoltzmannModeling”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FORTRAN90, Python, C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LB3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ccs.chem.ucl.ac.uk/lb3d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shan-Chen model for binary fluid interaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FORTRAN 90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LGPL version 3.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LBDEMcoupling-public</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017 – Jan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/ParticulateFlow/LBDEMcoupling-public</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coupling between the Lattice-Boltzmann code Palabos and the DEM code LIGGGHTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPLv3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LBSim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015 – Nov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/noirb/lbsim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supporting complex boundaries</t>
-  </si>
-  <si>
     <t xml:space="preserve">Limbes</t>
   </si>
   <si>
@@ -458,12 +500,36 @@
     <t xml:space="preserve">Cmake, VDKFortran</t>
   </si>
   <si>
+    <t xml:space="preserve">loliverhennigh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 – Feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/loliverhennigh/Lattice-Boltzmann-fluid-flow-in-Tensorflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">written in Tensorflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q5, D3Q15, D3Q19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ludwig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/ludwig-cf/ludwig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complex fluids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANSI C</t>
+  </si>
+  <si>
     <t xml:space="preserve">LUMA</t>
   </si>
   <si>
-    <t xml:space="preserve">2018 – Feb</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://github.com/ElsevierSoftwareX/SOFTX-D-18-00007</t>
   </si>
   <si>
@@ -473,6 +539,15 @@
     <t xml:space="preserve">C, C++</t>
   </si>
   <si>
+    <t xml:space="preserve">Mechsys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://mechsys.nongnu.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simulation tools in mechanics</t>
+  </si>
+  <si>
     <t xml:space="preserve">MP-LABS</t>
   </si>
   <si>
@@ -506,6 +581,9 @@
     <t xml:space="preserve">GNU GPL</t>
   </si>
   <si>
+    <t xml:space="preserve">openLBMflow</t>
+  </si>
+  <si>
     <t xml:space="preserve">Palabos</t>
   </si>
   <si>
@@ -524,6 +602,39 @@
     <t xml:space="preserve">GNU APGLV3</t>
   </si>
   <si>
+    <t xml:space="preserve">ParallelLbmCranfield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016 – Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/mate-szoke/ParallelLbmCranfield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parallel Lattice Boltzmann Method solver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUDA and PGAS UPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PowerFLOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.3ds.com/products-services/simulia/products/powerflow/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProLB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.prolb-cfd.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">highly complex flows</t>
+  </si>
+  <si>
     <t xml:space="preserve">pyLBM</t>
   </si>
   <si>
@@ -536,9 +647,6 @@
     <t xml:space="preserve">all in one package</t>
   </si>
   <si>
-    <t xml:space="preserve">1D, 2D, 3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">D1Q2, D1Q3, D2Q5, D2Q9, DQ15</t>
   </si>
   <si>
@@ -600,18 +708,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lattice Boltzmann code from LANL , Shan and Chen Lattice Boltzmann Method </t>
-  </si>
-  <si>
-    <t xml:space="preserve">loliverhennigh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/loliverhennigh/Lattice-Boltzmann-fluid-flow-in-Tensorflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">written in Tensorflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2Q5, D3Q15, D3Q19</t>
   </si>
   <si>
     <t xml:space="preserve">turbulent_lbm_multigpu</t>
@@ -680,7 +776,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="165" formatCode="YY/MM/DD"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -805,12 +901,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -826,7 +922,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -843,18 +939,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ36"/>
+  <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.04"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,24 +1258,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="D8" s="0" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>69</v>
@@ -1183,64 +1280,51 @@
       <c r="H8" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="L8" s="5"/>
+      <c r="N8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="R8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="M8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>25</v>
+      <c r="L9" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R9" s="0" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -1248,220 +1332,226 @@
         <v>79</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="E10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="H10" s="0" t="s">
-        <v>70</v>
-      </c>
       <c r="L10" s="0" t="s">
-        <v>24</v>
+        <v>83</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>86</v>
+        <v>3</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>208</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>2020</v>
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="R12" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>2017</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>97</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>7</v>
+        <v>208</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="M14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R14" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="N14" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="R14" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>106</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>20</v>
+        <v>2017</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="L15" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>112</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>22</v>
@@ -1470,176 +1560,181 @@
         <v>23</v>
       </c>
       <c r="L16" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="M16" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="N16" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="N16" s="0" t="s">
-        <v>115</v>
-      </c>
       <c r="R16" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="0" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="E17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>2016</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="L17" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="H17" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>121</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>2012</v>
+      </c>
       <c r="D18" s="0" t="s">
         <v>122</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>123</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="L18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="E19" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="H19" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="L19" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="N19" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="E20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="H20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L20" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="M20" s="5"/>
+      <c r="N20" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C21" s="0" t="n">
-        <v>2014</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="E21" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E21" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G21" s="5" t="s">
+      <c r="L21" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>40</v>
-      </c>
+      <c r="M21" s="5"/>
       <c r="N21" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
@@ -1653,31 +1748,13 @@
         <v>140</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="N22" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="R22" s="0" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,72 +1762,75 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>146</v>
+        <v>18</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>2019</v>
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="I23" s="0" t="s">
+        <v>23</v>
+      </c>
       <c r="L23" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>147</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>152</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="M24" s="0" t="s">
         <v>40</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="R24" s="0" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,154 +1838,133 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>158</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>38</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>159</v>
+        <v>62</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>24</v>
+        <v>156</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>160</v>
+        <v>40</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>157</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>163</v>
-      </c>
       <c r="E26" s="0" t="n">
-        <v>672</v>
+        <v>4</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>2020</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>164</v>
+      <c r="G26" s="0" t="s">
+        <v>162</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>165</v>
+      <c r="I26" s="0" t="s">
+        <v>163</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M26" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="N26" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="L27" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="L27" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="M27" s="0" t="s">
-        <v>173</v>
-      </c>
       <c r="N27" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R27" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>178</v>
+        <v>2019</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>170</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="R28" s="0" t="s">
-        <v>181</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,252 +1972,529 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>59</v>
+        <v>172</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>70</v>
+        <v>38</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>118</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="R30" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>27</v>
+        <v>200</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>192</v>
+        <v>2020</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>183</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>38</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>107</v>
+        <v>184</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>124</v>
+        <v>24</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>185</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="L32" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>20</v>
+        <v>672</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>2020</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>200</v>
+        <v>190</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>191</v>
       </c>
       <c r="L33" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M33" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="O33" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M33" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>50</v>
+        <v>194</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>454</v>
+        <v>1</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="L34" s="0" t="s">
-        <v>72</v>
+        <v>22</v>
+      </c>
+      <c r="I34" s="5"/>
+      <c r="L34" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>40</v>
+        <v>198</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R34" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="L35" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>200</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="N37" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R37" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C38" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="D38" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="E38" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H38" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="M38" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="H36" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="L36" s="0" t="s">
+      <c r="N38" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="M36" s="0" t="s">
-        <v>109</v>
+      <c r="R38" s="0" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="M40" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="O42" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N43" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R43" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L45" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="M45" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>